<commit_message>
Updated Chinese Wall template
</commit_message>
<xml_diff>
--- a/src/Chinese wall/Import/CW_check - Template.xlsx
+++ b/src/Chinese wall/Import/CW_check - Template.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WZHARBC\Documents\repos\monthly_tasks\src\Chinese wall\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9AA801-2B3C-4E49-9EFC-5AAA62AFA4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD84B5A9-98A4-4026-A71F-8F4103346034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{28F8725F-EB40-496F-8BA0-68FD3C4454F9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="102">
   <si>
     <t>ws</t>
   </si>
@@ -119,9 +119,6 @@
     <t>COSME_RBBG_2016_NR</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>JE1_BG_NR</t>
   </si>
   <si>
@@ -339,6 +336,15 @@
   </si>
   <si>
     <t>ROOF_CORP_2022_HR_NR, ROOF_HUNGARY_2O22_1, ROOF_RBRO_2022_NR</t>
+  </si>
+  <si>
+    <t>Other "NR"</t>
+  </si>
+  <si>
+    <t>Other "RE"</t>
+  </si>
+  <si>
+    <t>1 only for: ROOF_CORP_2021_RBIAG_NR, ROOF_CORP_2022_RBIAG_NR, ROOF_CRE_2019_RBIAG_NR</t>
   </si>
 </sst>
 </file>
@@ -2963,11 +2969,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AFB7FDD-A7E8-44C8-BEBA-605CAE21C641}">
-  <dimension ref="A1:Y89"/>
+  <dimension ref="A1:AC89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="56" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O22" sqref="O22"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3020,7 +3026,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -3034,7 +3040,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>6</v>
@@ -3051,13 +3057,13 @@
         <v>15</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>11</v>
@@ -3083,16 +3089,16 @@
         <v>15</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -3130,16 +3136,16 @@
         <v>15</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -3167,16 +3173,16 @@
         <v>15</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H7" s="3">
         <v>1</v>
@@ -3186,7 +3192,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="Q7" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R7" s="7">
         <v>1</v>
@@ -3206,13 +3212,13 @@
         <v>15</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>9</v>
@@ -3223,7 +3229,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="Q8" s="7" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="R8" s="7">
         <v>1</v>
@@ -3247,13 +3253,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>19</v>
@@ -3265,19 +3271,34 @@
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="3"/>
+      <c r="Q9" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="R9" s="7">
+        <v>1</v>
+      </c>
+      <c r="S9" s="7">
+        <v>1</v>
+      </c>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>80</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>10</v>
@@ -3291,28 +3312,24 @@
       <c r="L10" s="3"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
-      <c r="Q10" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="R10" s="13" t="s">
-        <v>28</v>
-      </c>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="13"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H11" s="3">
         <v>1</v>
@@ -3322,10 +3339,10 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="Q11" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R11" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -3342,7 +3359,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H12" s="3">
         <v>1</v>
@@ -3352,10 +3369,10 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="Q12" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R12" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -3372,7 +3389,7 @@
         <v>19</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
@@ -3382,10 +3399,10 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="Q13" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="R13" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -3399,7 +3416,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>22</v>
@@ -3410,10 +3427,10 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="Q14" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="R14" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -3427,7 +3444,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>23</v>
@@ -3439,6 +3456,12 @@
       <c r="J15" s="17"/>
       <c r="K15" s="17"/>
       <c r="L15" s="3"/>
+      <c r="Q15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="R15" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -3451,7 +3474,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>25</v>
@@ -3464,7 +3487,7 @@
       <c r="K16" s="17"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3475,10 +3498,10 @@
         <v>5</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H17" s="3">
         <v>1</v>
@@ -3488,7 +3511,7 @@
       <c r="K17" s="17"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3499,10 +3522,10 @@
         <v>5</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H18" s="3">
         <v>1</v>
@@ -3511,8 +3534,13 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="W18" s="16"/>
+      <c r="Z18" s="16"/>
+      <c r="AC18" s="16"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3526,7 +3554,7 @@
         <v>23</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H19" s="3">
         <v>1</v>
@@ -3535,8 +3563,13 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="W19" s="16"/>
+      <c r="Z19" s="16"/>
+      <c r="AC19" s="16"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3550,7 +3583,7 @@
         <v>25</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H20" s="3">
         <v>1</v>
@@ -3559,8 +3592,13 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="W20" s="16"/>
+      <c r="Z20" s="16"/>
+      <c r="AC20" s="16"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3571,10 +3609,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" s="3">
         <v>1</v>
@@ -3583,9 +3621,13 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="R21" s="3"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="W21" s="16"/>
+      <c r="Z21" s="16"/>
+      <c r="AC21" s="16"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3596,10 +3638,10 @@
         <v>5</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H22" s="3">
         <v>1</v>
@@ -3608,9 +3650,13 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="R22" s="3"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="W22" s="16"/>
+      <c r="Z22" s="16"/>
+      <c r="AC22" s="16"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -3621,10 +3667,10 @@
         <v>5</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H23" s="3">
         <v>1</v>
@@ -3633,9 +3679,13 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="R23" s="3"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="Z23" s="16"/>
+      <c r="AC23" s="16"/>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3646,10 +3696,10 @@
         <v>5</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H24" s="3">
         <v>1</v>
@@ -3658,9 +3708,13 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="R24" s="3"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="W24" s="16"/>
+      <c r="Z24" s="16"/>
+      <c r="AC24" s="16"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -3671,10 +3725,10 @@
         <v>5</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H25" s="3">
         <v>1</v>
@@ -3683,9 +3737,13 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="R25" s="3"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="Z25" s="16"/>
+      <c r="AC25" s="16"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -3696,10 +3754,10 @@
         <v>5</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H26" s="3">
         <v>1</v>
@@ -3714,8 +3772,13 @@
       <c r="L26" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="Z26" s="16"/>
+      <c r="AC26" s="16"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3726,10 +3789,10 @@
         <v>5</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H27" s="3">
         <v>1</v>
@@ -3740,8 +3803,13 @@
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="Z27" s="16"/>
+      <c r="AC27" s="16"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -3752,18 +3820,23 @@
         <v>5</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="W28" s="16"/>
+      <c r="Z28" s="16"/>
+      <c r="AC28" s="16"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -3774,10 +3847,10 @@
         <v>5</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H29" s="3">
         <v>1</v>
@@ -3788,22 +3861,24 @@
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q29" s="12"/>
+      <c r="R29" s="13"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H30" s="3">
         <v>1</v>
@@ -3815,22 +3890,24 @@
       <c r="K30" s="19"/>
       <c r="L30" s="3"/>
       <c r="P30" s="16"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q30" s="12"/>
+      <c r="R30" s="13"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>59</v>
-      </c>
       <c r="G31" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H31" s="3">
         <v>1</v>
@@ -3843,21 +3920,21 @@
       <c r="L31" s="3"/>
       <c r="P31" s="16"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H32" s="3">
         <v>1</v>
@@ -3875,16 +3952,16 @@
         <v>12</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H33" s="3">
         <v>1</v>
@@ -3902,16 +3979,16 @@
         <v>12</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H34" s="3">
         <v>1</v>
@@ -3935,16 +4012,16 @@
         <v>12</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -3958,16 +4035,16 @@
         <v>12</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H36" s="3">
         <v>1</v>
@@ -3989,16 +4066,16 @@
         <v>12</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H37" s="3">
         <v>1</v>
@@ -4016,16 +4093,16 @@
         <v>12</v>
       </c>
       <c r="B38" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>84</v>
-      </c>
       <c r="G38" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H38" s="3">
         <v>5</v>
@@ -4041,16 +4118,16 @@
         <v>12</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -4064,16 +4141,16 @@
         <v>12</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H40" s="3">
         <v>1</v>
@@ -4091,16 +4168,16 @@
         <v>12</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H41" s="3">
         <v>1</v>
@@ -4118,16 +4195,16 @@
         <v>12</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C42" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H42" s="3">
         <v>1</v>
@@ -4143,16 +4220,16 @@
         <v>12</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C43" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H43" s="3">
         <v>1</v>
@@ -4168,16 +4245,16 @@
         <v>12</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -4191,16 +4268,16 @@
         <v>12</v>
       </c>
       <c r="B45" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>91</v>
-      </c>
       <c r="G45" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H45" s="3">
         <v>1</v>
@@ -4216,16 +4293,16 @@
         <v>12</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C46" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H46" s="3">
         <v>1</v>
@@ -4241,16 +4318,16 @@
         <v>12</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -4264,16 +4341,16 @@
         <v>12</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="H48" s="3">
         <v>1</v>
@@ -4289,16 +4366,16 @@
         <v>12</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C49" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H49" s="3">
         <v>1</v>
@@ -4314,16 +4391,16 @@
         <v>12</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C50" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H50" s="3">
         <v>1</v>
@@ -4339,16 +4416,16 @@
         <v>12</v>
       </c>
       <c r="B51" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>32</v>
-      </c>
       <c r="G51" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H51" s="3">
         <v>1</v>
@@ -4364,16 +4441,16 @@
         <v>12</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H52" s="3">
         <v>1</v>
@@ -4389,16 +4466,16 @@
         <v>12</v>
       </c>
       <c r="B53" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>98</v>
-      </c>
       <c r="G53" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H53" s="3">
         <v>1</v>
@@ -4414,16 +4491,16 @@
         <v>12</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
@@ -4437,16 +4514,16 @@
         <v>12</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C55" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H55" s="3">
         <v>1</v>
@@ -4462,16 +4539,16 @@
         <v>12</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C56" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
@@ -4485,16 +4562,16 @@
         <v>12</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H57" s="3">
         <v>1</v>
@@ -4510,16 +4587,16 @@
         <v>13</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H58" s="3">
         <v>1</v>
@@ -4535,16 +4612,16 @@
         <v>13</v>
       </c>
       <c r="B59" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>59</v>
-      </c>
       <c r="G59" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H59" s="3">
         <v>48</v>
@@ -4568,13 +4645,13 @@
         <v>13</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C60" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P60" s="16"/>
     </row>
@@ -4583,13 +4660,13 @@
         <v>13</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C61" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P61" s="16"/>
     </row>
@@ -4598,13 +4675,13 @@
         <v>13</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C62" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P62" s="16"/>
     </row>
@@ -4619,7 +4696,7 @@
         <v>5</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P63" s="16"/>
     </row>
@@ -4628,13 +4705,13 @@
         <v>14</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C64" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P64" s="16"/>
     </row>
@@ -4643,13 +4720,13 @@
         <v>14</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C65" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P65" s="16"/>
     </row>
@@ -4664,7 +4741,7 @@
         <v>5</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P66" s="16"/>
     </row>
@@ -4673,13 +4750,13 @@
         <v>17</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C67" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P67" s="16"/>
     </row>
@@ -4688,13 +4765,13 @@
         <v>17</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C68" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P68" s="16"/>
     </row>
@@ -4733,7 +4810,7 @@
       <c r="C74" s="16"/>
       <c r="D74" s="16"/>
       <c r="G74" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -4741,7 +4818,7 @@
       <c r="C75" s="16"/>
       <c r="D75" s="16"/>
       <c r="G75" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H75" s="1"/>
     </row>
@@ -4751,10 +4828,10 @@
       <c r="D76" s="16"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -4763,11 +4840,11 @@
       <c r="D77" s="16"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I77" s="1"/>
       <c r="L77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -4776,11 +4853,11 @@
       <c r="D78" s="16"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I78" s="1"/>
       <c r="L78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -4788,11 +4865,11 @@
       <c r="C79" s="16"/>
       <c r="D79" s="16"/>
       <c r="H79" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I79" s="1"/>
       <c r="L79" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -4801,11 +4878,11 @@
       <c r="D80" s="16"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I80" s="1"/>
       <c r="L80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
@@ -4814,11 +4891,11 @@
       <c r="D81" s="16"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I81" s="1"/>
       <c r="L81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
@@ -4826,60 +4903,60 @@
       <c r="C82" s="16"/>
       <c r="D82" s="16"/>
       <c r="H82" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I82" s="1"/>
       <c r="L82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H83" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I83" s="1"/>
       <c r="L83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G84" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G85" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G86" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G87" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G88" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G89" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -4890,31 +4967,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Gruppe xmlns="86cedade-ebff-4b8d-b2a3-faad7f3c3397">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Gruppe>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100744D2F48F15A9F42AB29E4A68231D9A4" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="076da6730c833006e4daab9ba0d81abb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="86cedade-ebff-4b8d-b2a3-faad7f3c3397" xmlns:ns3="916002f9-0322-485a-9445-426815c01027" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df2694061866efa02c56035bac5f9ae1" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5168,33 +5220,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFA003BC-8A43-4088-A486-A3327AB89D31}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="916002f9-0322-485a-9445-426815c01027"/>
-    <ds:schemaRef ds:uri="86cedade-ebff-4b8d-b2a3-faad7f3c3397"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF6A3DD9-A393-474B-8508-3F40507D28E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Gruppe xmlns="86cedade-ebff-4b8d-b2a3-faad7f3c3397">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Gruppe>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EF533D6-B144-4ECA-9EA2-FEA5FE866A02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5212,4 +5263,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF6A3DD9-A393-474B-8508-3F40507D28E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFA003BC-8A43-4088-A486-A3327AB89D31}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="916002f9-0322-485a-9445-426815c01027"/>
+    <ds:schemaRef ds:uri="86cedade-ebff-4b8d-b2a3-faad7f3c3397"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>